<commit_message>
added 'replace existing' column to sequence upload file;
</commit_message>
<xml_diff>
--- a/data/files/mschool_sequences_template.xlsx
+++ b/data/files/mschool_sequences_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>First Name</t>
   </si>
@@ -46,18 +46,35 @@
   </si>
   <si>
     <t>5th</t>
+  </si>
+  <si>
+    <t>Replace Existing</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstGrowiReady</t>
+  </si>
+  <si>
+    <t>987659</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lau</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brigette</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="5">
     <font>
       <sz val="12"/>
@@ -452,19 +469,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="9" width="17.1640625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="10" width="17.1640625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,25 +492,46 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
removed testing data from sequence upload template;
</commit_message>
<xml_diff>
--- a/data/files/mschool_sequences_template.xlsx
+++ b/data/files/mschool_sequences_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>First Name</t>
   </si>
@@ -49,25 +49,6 @@
   </si>
   <si>
     <t>Replace Existing</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>FirstGrowiReady</t>
-  </si>
-  <si>
-    <t>987659</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lau</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brigette</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -469,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -513,25 +494,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>